<commit_message>
Added new preparation medium and storage medium
Closes #30 and closes #31
</commit_message>
<xml_diff>
--- a/sample-suspension/latest/sample-suspension.xlsx
+++ b/sample-suspension/latest/sample-suspension.xlsx
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="150">
   <si>
     <t>source_id</t>
   </si>
@@ -304,6 +304,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000126</t>
   </si>
   <si>
+    <t>Alpha-MEM</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000371</t>
+  </si>
+  <si>
     <t>2% PFA/2.5% Glutaraldehyde</t>
   </si>
   <si>
@@ -340,6 +346,12 @@
     <t>http://purl.obolibrary.org/obo/CHEBI_16236</t>
   </si>
   <si>
+    <t>Modified Davidson's Fixative</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000370</t>
+  </si>
+  <si>
     <t>Inflated (Agarose)</t>
   </si>
   <si>
@@ -370,6 +382,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000198</t>
   </si>
   <si>
+    <t>Growth media</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000372</t>
+  </si>
+  <si>
     <t>RNAlater</t>
   </si>
   <si>
@@ -400,6 +418,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000147</t>
   </si>
   <si>
+    <t>Lysis buffer</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C178573</t>
+  </si>
+  <si>
     <t>preparation_condition</t>
   </si>
   <si>
@@ -460,6 +484,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C63523</t>
   </si>
   <si>
+    <t>Formic acid in water</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C83719</t>
+  </si>
+  <si>
     <t>DMSO (no serum)</t>
   </si>
   <si>
@@ -574,7 +604,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-03-18T09:39:12-07:00</t>
+    <t>2024-04-20T17:32:34-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -727,45 +757,45 @@
         <v>26</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2">
       <c r="U2" t="s" s="22">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -785,7 +815,7 @@
       <formula1>'tissue_weight_unit'!$A$1:$A$4</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_medium'!$A$1:$A$26</formula1>
+      <formula1>'preparation_medium'!$A$1:$A$30</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="J2:J1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'preparation_condition'!$A$1:$A$8</formula1>
@@ -798,7 +828,7 @@
       <formula1>'processing_time_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="M2:M1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'storage_medium'!$A$1:$A$20</formula1>
+      <formula1>'storage_medium'!$A$1:$A$21</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="N2:N1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'storage_method'!$A$1:$A$11</formula1>
@@ -830,12 +860,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -859,30 +889,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -990,7 +1020,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1202,6 +1232,38 @@
       </c>
       <c r="B26" t="s" s="0">
         <v>78</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>81</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1219,34 +1281,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5">
@@ -1259,26 +1321,26 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1325,7 +1387,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1333,18 +1395,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3">
@@ -1357,10 +1419,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
@@ -1373,114 +1435,114 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>64</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>40</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>102</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>44</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>104</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>70</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>75</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>76</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>48</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20">
@@ -1489,6 +1551,14 @@
       </c>
       <c r="B20" t="s" s="0">
         <v>54</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1506,34 +1576,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5">
@@ -1546,50 +1616,50 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>115</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1607,18 +1677,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'Concentrated quench buffer' in the storage_medium
Closes #49
</commit_message>
<xml_diff>
--- a/sample-suspension/latest/sample-suspension.xlsx
+++ b/sample-suspension/latest/sample-suspension.xlsx
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="156">
   <si>
     <t>source_id</t>
   </si>
@@ -508,6 +508,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000135</t>
   </si>
   <si>
+    <t>Concentrated quench buffer</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000391</t>
+  </si>
+  <si>
     <t>Gelatin</t>
   </si>
   <si>
@@ -616,7 +622,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-06-28T15:48:18-07:00</t>
+    <t>2024-10-02T11:08:45-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -781,33 +787,33 @@
         <v>106</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2">
       <c r="U2" t="s" s="22">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +846,7 @@
       <formula1>'processing_time_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="M2:M1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'storage_medium'!$A$1:$A$22</formula1>
+      <formula1>'storage_medium'!$A$1:$A$23</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="N2:N1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'storage_method'!$A$1:$A$12</formula1>
@@ -872,12 +878,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -901,30 +907,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1407,7 +1413,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1503,18 +1509,18 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>44</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>115</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>116</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14">
@@ -1535,18 +1541,18 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>77</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>78</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>122</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
@@ -1559,33 +1565,41 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>83</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>84</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>50</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="B22" t="s" s="0">
+      <c r="B23" t="s" s="0">
         <v>56</v>
       </c>
     </row>
@@ -1644,26 +1658,26 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9">
@@ -1713,18 +1727,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add water as a storage medium
Closes #123
</commit_message>
<xml_diff>
--- a/sample-suspension/latest/sample-suspension.xlsx
+++ b/sample-suspension/latest/sample-suspension.xlsx
@@ -30,130 +30,147 @@
   <commentList>
     <comment ref="A1" authorId="1">
       <text>
-        <t>(Required) Unique HuBMAP or SenNet identifier for the source (parent) from which
-the sample was taken. Example: HBM122.EFGH.789 or SNT234.RTYU.119</t>
+        <t>(Required) The unique identifier from HuBMAP or SenNet for the source (parent
+data) from which the sample was derived. Example: HBM122.EFGH.789</t>
       </text>
     </comment>
     <comment ref="B1" authorId="1">
       <text>
-        <t>(Required) Unique HuBMAP or SenNet identifier for the sample assigned by the
-ingest portal. Example: HBM743.CKJW.876 or SNT923.UYTE.122</t>
+        <t>(Required) The unique HuBMAP or SenNet identifier assigned to the sample by the
+ingest portal. Example: HBM743.CKJW.876</t>
       </text>
     </comment>
     <comment ref="C1" authorId="1">
       <text>
-        <t>An internal field labs can use it to add whatever ID(s) they want or need for
-dataset validation and tracking. This could be a single ID (e.g.,
-"Visium_9OLC_A4_S1") or a delimited list of IDs (e.g., “9OL; 9OLC.A2;
-Visium_9OLC_A4_S1”). This field will not be accessible to anyone outside of the
-consortium and no effort will be made to check if IDs provided by one data
-provider are also used by another.</t>
+        <t>A locally assigned identifier provided by the data provider for the dataset. It
+is used to reference an external metadata record that may be maintained
+independently, enabling traceability and supporting provenance tracking.
+Example: Visium_9OLC_A4_S1</t>
       </text>
     </comment>
     <comment ref="D1" authorId="1">
       <text>
-        <t>(Required) DOI for the protocols.io page that describes the assay or sample
-procurement and preparation. For example for an imaging assay, the protocol
-might begin with staining of a section and finalize with the creation of an
-OME-TIFF file. In this case the protocol would include any image processing
-steps required to create the OME-TIFF file. Example:
-https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1.</t>
+        <t>(Required) The DOI for the protocols.io page that details the assay or the
+procedures used for sample procurement and preparation. For example, in the case
+of an imaging assay, the protocol may start with tissue section staining and end
+with the generation of an OME-TIFF file. The documented protocol should also
+include any image processing steps involved in producing the final OME-TIFF.
+Example: https://dx.doi.org/10.17504/protocols.io.eq2lyno9qvx9/v1</t>
       </text>
     </comment>
     <comment ref="E1" authorId="1">
       <text>
-        <t>(Required) How long was the source material (parent) stored, prior to this
-sample being processed.</t>
+        <t>(Required) The length of time the sample was stored prior to processing it. For
+assays performed on tissue sections, this refers to how long the tissue section
+(e.g., slide) was stored before the assay began (e.g., imaging). For assays
+performed on suspensions, such as sequencing, it refers to how long the
+suspension was stored before library construction started. Example: 12</t>
       </text>
     </comment>
     <comment ref="F1" authorId="1">
       <text>
-        <t>(Required) The time duration unit of measurement</t>
+        <t>(Required) The unit of measurement used to specify the source storage duration
+value. Example: hour</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1">
       <text>
-        <t>The weight of a tissue block or the piece of tissue used in a suspension.
-Knowing the weight of the parent block and tissue used in a suspension, allows
-us to compute what percentage of the block was used for the suspension.</t>
+        <t>The weight of a tissue block or the piece of tissue used in a suspension. This
+information is crucial for calculating the percentage of the parent block that
+was utilized in the suspension preparation. If the weight is not applicable or
+unknown, this field may be left blank. Example: 100</t>
       </text>
     </comment>
     <comment ref="H1" authorId="1">
       <text>
-        <t>The tissue weight unit of measurement</t>
+        <t>The unit of measurement for the tissue weight value. If no tissue weight is
+specified, this field may be left blank. Example: g</t>
       </text>
     </comment>
     <comment ref="I1" authorId="1">
       <text>
-        <t>(Required) The medium used during the sample preparation</t>
+        <t>(Required) The medium used during the sample preparation process. If no specific
+medium was utilized, enter "None". If medium was not recorded, enter "Unknown".
+Example: Fresh frozen CMC</t>
       </text>
     </comment>
     <comment ref="J1" authorId="1">
       <text>
-        <t>(Required) The condition by which the preparation occurred, such as was the
-sample placed in dry ice during the preparation.</t>
+        <t>(Required) The condition under which the sample preparation took place, such as
+whether the sample was placed on dry ice during the process. If preparation
+condition was not recorded, enter "Unknown". Example: Frozen on dry ice</t>
       </text>
     </comment>
     <comment ref="K1" authorId="1">
       <text>
-        <t>How long the tissue was being handled before the initial preservation</t>
+        <t>The duration for which the tissue was handled prior to its initial preservation.
+Example: 120</t>
       </text>
     </comment>
     <comment ref="L1" authorId="1">
       <text>
-        <t>The time unit of measurement</t>
+        <t>The unit of measurement for the processing time value. If processing time is not
+specified, this field may be left blank. Example: minute</t>
       </text>
     </comment>
     <comment ref="M1" authorId="1">
       <text>
-        <t>(Required) What was the sample preserved in.</t>
+        <t>(Required) The medium used to preserve the sample. If no specific medium was
+utilized, enter "None". If medium was not recorded, enter "Unknown". Example:
+FFPE (Paraffin embedded)</t>
       </text>
     </comment>
     <comment ref="N1" authorId="1">
       <text>
-        <t>(Required) The method by which the sample was stored, after preparation and
-before the assay was performed.</t>
+        <t>(Required) The method used to store the sample after preparation and prior to
+performing the assay. If no specific storage method was utilized, enter "None".
+If storage method was not recorded, enter "Unknown". Example: Frozen in dry ice</t>
       </text>
     </comment>
     <comment ref="O1" authorId="1">
       <text>
-        <t>For example, RIN: 8.7. For suspensions, measured by visual inspection prior to
-cell lysis or defined by known parameters such as wells with several cells or no
-cells. This can be captured at a high level. "OK" or "not OK", or with more
-specificity such as "debris", "clump", "low clump".</t>
+        <t>The quality criteria used to assess the sample, which may include metrics such
+as RIN (e.g., RIN: 8.7) or visual inspection parameters for suspensions prior to
+cell lysis. These criteria can be captured at a high level with general terms
+like "OK" or "not OK" or with more specific descriptors such as "debris" "clump"
+or "low clump". Example: RIN: 8.7, low clump, no visible debris</t>
       </text>
     </comment>
     <comment ref="P1" authorId="1">
       <text>
-        <t>(Required) The type of single cell entity derived from isolation protocol.</t>
+        <t>(Required) The type of single-cell entity that is derived from the isolation
+protocol. Example: Nucleus + cell</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>(Required) Total number of cell/nuclei yielded post dissociation and enrichment.</t>
+        <t>(Required) The total number of cells or nuclei obtained following the processes
+of dissociation and enrichment. Example: 300000</t>
       </text>
     </comment>
     <comment ref="R1" authorId="1">
       <text>
-        <t>(Required) Was the cell/nuclei population enriched?</t>
+        <t>(Required) Indicates whether the cell or nuclei population was enriched prior to
+analysis. Example: Yes</t>
       </text>
     </comment>
     <comment ref="S1" authorId="1">
       <text>
-        <t>If the suspension was enriched, then this is the target of the enrichment.</t>
+        <t>The target of enrichment if the suspension was enriched. Example: CD8+ T cells</t>
       </text>
     </comment>
     <comment ref="T1" authorId="1">
       <text>
-        <t>Miscellaneous details about the sample, not captured in the existing metadata
-fields.</t>
+        <t>Miscellaneous details about the sample that are not captured in the existing
+metadata fields. Example: Sample was stored at 4°C for 48 hours prior to
+processing due to equipment maintenance delay</t>
       </text>
     </comment>
     <comment ref="U1" authorId="1">
       <text>
-        <t>(Required) The string that serves as the definitive identifier for the metadata
-schema version and is readily interpretable by computers for data validation and
-processing.</t>
+        <t>(Required) The unique string identifier for the metadata specification version,
+which is easily interpretable by computers for purposes of data validation and
+processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
       </text>
     </comment>
   </commentList>
@@ -161,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="164">
   <si>
     <t>source_id</t>
   </si>
@@ -490,30 +507,54 @@
     <t>storage_medium</t>
   </si>
   <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65147</t>
+  </si>
+  <si>
+    <t>OCT</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C63523</t>
+  </si>
+  <si>
+    <t>DMSO (no serum)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000115</t>
+  </si>
+  <si>
+    <t>Gelatin</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65802</t>
+  </si>
+  <si>
+    <t>DMSO (serum)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000125</t>
+  </si>
+  <si>
+    <t>CMC</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C83594</t>
+  </si>
+  <si>
     <t>1X quench buffer</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000427</t>
   </si>
   <si>
-    <t>OCT</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C63523</t>
-  </si>
-  <si>
     <t>Formic acid in water</t>
   </si>
   <si>
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C83719</t>
   </si>
   <si>
-    <t>DMSO (no serum)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000115</t>
-  </si>
-  <si>
     <t>Tris-EDTA</t>
   </si>
   <si>
@@ -526,36 +567,18 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000391</t>
   </si>
   <si>
-    <t>Gelatin</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C65802</t>
-  </si>
-  <si>
     <t>Cryo-EM</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000333</t>
   </si>
   <si>
-    <t>DMSO (serum)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000125</t>
-  </si>
-  <si>
     <t>FFPE (Paraffin embedded)</t>
   </si>
   <si>
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C143028</t>
   </si>
   <si>
-    <t>CMC</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C83594</t>
-  </si>
-  <si>
     <t>storage_method</t>
   </si>
   <si>
@@ -640,7 +663,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-04-24T10:45:49-07:00</t>
+    <t>2025-10-16T07:27:53-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -805,33 +828,33 @@
         <v>108</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2">
       <c r="U2" t="s" s="22">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -864,7 +887,7 @@
       <formula1>'processing_time_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="M2:M1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'storage_medium'!$A$1:$A$24</formula1>
+      <formula1>'storage_medium'!$A$1:$A$25</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="N2:N1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'storage_method'!$A$1:$A$12</formula1>
@@ -896,12 +919,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -925,30 +948,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1439,7 +1462,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1447,114 +1470,114 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>60</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>111</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>112</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>62</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>114</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>66</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>71</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>72</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>117</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>118</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>119</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>120</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15">
@@ -1567,74 +1590,82 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>123</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>124</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>127</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>128</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>86</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>52</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>56</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>58</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1692,26 +1723,26 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9">
@@ -1761,26 +1792,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a new storage medium: Nuclease-free water
Closes #147
</commit_message>
<xml_diff>
--- a/sample-suspension/latest/sample-suspension.xlsx
+++ b/sample-suspension/latest/sample-suspension.xlsx
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="174">
   <si>
     <t>source_id</t>
   </si>
@@ -567,6 +567,12 @@
     <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C83594</t>
   </si>
   <si>
+    <t>Nuclease-free water</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000482</t>
+  </si>
+  <si>
     <t>1X quench buffer</t>
   </si>
   <si>
@@ -687,7 +693,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-11-03T17:32:07-08:00</t>
+    <t>2026-02-24T15:31:04-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -852,33 +858,33 @@
         <v>116</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2">
       <c r="U2" t="s" s="22">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -911,7 +917,7 @@
       <formula1>'processing_time_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="M2:M1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'storage_medium'!$A$1:$A$25</formula1>
+      <formula1>'storage_medium'!$A$1:$A$26</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="N2:N1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'storage_method'!$A$1:$A$12</formula1>
@@ -943,12 +949,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -972,30 +978,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1518,7 +1524,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1606,82 +1612,82 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>56</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>129</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>130</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>66</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>131</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>132</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>69</v>
+        <v>133</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>70</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>133</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>134</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21">
@@ -1702,25 +1708,33 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>85</v>
+        <v>139</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>86</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>140</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="B25" t="s" s="0">
+      <c r="B26" t="s" s="0">
         <v>92</v>
       </c>
     </row>
@@ -1779,26 +1793,26 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9">
@@ -1848,26 +1862,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>